<commit_message>
Establece nombre de columnas y llamada de celdas de excel
</commit_message>
<xml_diff>
--- a/Controller/data.xlsx
+++ b/Controller/data.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\PycharmProjects\Oil-Apps\PVT_Proyectsoft\Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E213A3-41D1-4F8B-BC99-EED342BA02FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7BDEED-0506-4282-9B67-4AFCB6993291}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Rs</t>
   </si>
@@ -66,19 +66,37 @@
     <t>Bo</t>
   </si>
   <si>
-    <t>Standing</t>
-  </si>
-  <si>
-    <t>Marhouns</t>
-  </si>
-  <si>
-    <t>Beals</t>
-  </si>
-  <si>
-    <t>Vaszques_Beggs</t>
-  </si>
-  <si>
-    <t>Correlacion lab</t>
+    <t>Rs_Standing</t>
+  </si>
+  <si>
+    <t>Rs_Marhouns</t>
+  </si>
+  <si>
+    <t>Bo_Standing</t>
+  </si>
+  <si>
+    <t>Bo_Marhouns</t>
+  </si>
+  <si>
+    <t>Pb_Standing</t>
+  </si>
+  <si>
+    <t>Pb_Marhouns</t>
+  </si>
+  <si>
+    <t>Uo_Beals</t>
+  </si>
+  <si>
+    <t>Po_Standing</t>
+  </si>
+  <si>
+    <t>Co_Standing</t>
+  </si>
+  <si>
+    <t>Co_Vaszques</t>
+  </si>
+  <si>
+    <t>Po_corre_lab</t>
   </si>
 </sst>
 </file>
@@ -143,19 +161,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,14 +474,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CED51A5-5DD9-425B-AE82-86A73D7AA283}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
     <col min="16" max="16" width="17.28515625" customWidth="1"/>
     <col min="18" max="18" width="21.42578125" customWidth="1"/>
   </cols>
@@ -494,73 +512,73 @@
         <v>9</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="4" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3" t="s">
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="3"/>
+      <c r="R1" s="2"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>853.22688958445372</v>
+        <v>1067.2188584748965</v>
       </c>
       <c r="C2">
-        <v>120.60894887441285</v>
+        <v>655.11397796629035</v>
       </c>
       <c r="D2">
-        <v>276.7842589621568</v>
+        <v>184.43771426267071</v>
       </c>
       <c r="E2">
-        <v>23.07522694522326</v>
+        <v>27.87872836230968</v>
       </c>
       <c r="F2">
-        <v>0.74012470252178353</v>
-      </c>
-      <c r="H2" s="5" t="s">
+        <v>0.71683002304553689</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="4" t="s">
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>13</v>
+      <c r="M2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -568,602 +586,602 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1203.3888831671059</v>
+        <v>5181.3404534776955</v>
       </c>
       <c r="C3">
-        <v>347.4008983826846</v>
+        <v>171.81136567441095</v>
       </c>
       <c r="D3">
-        <v>166.52758986210134</v>
+        <v>272.06986763096648</v>
       </c>
       <c r="E3">
-        <v>36.712252673341325</v>
+        <v>20.821987733516899</v>
       </c>
       <c r="F3">
-        <v>0.65320406448146939</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
+        <v>0.69155355073649738</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>2542.795134363917</v>
+        <v>4429.1843926359616</v>
       </c>
       <c r="C4">
-        <v>315.25917045064432</v>
+        <v>800</v>
       </c>
       <c r="D4">
-        <v>348.65915092921415</v>
+        <v>171.22915513732767</v>
       </c>
       <c r="E4">
-        <v>29.788451092324284</v>
+        <v>36.389787415894396</v>
       </c>
       <c r="F4">
-        <v>0.72008831511935312</v>
-      </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+        <v>0.73286681896504835</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4292.5138602765765</v>
+        <v>5226.1246704571531</v>
       </c>
       <c r="C5">
-        <v>470.42479771662704</v>
+        <v>490.77964112763004</v>
       </c>
       <c r="D5">
-        <v>212.56570291267286</v>
+        <v>344.61667329065057</v>
       </c>
       <c r="E5">
-        <v>25.972774739592921</v>
+        <v>35.634298239153111</v>
       </c>
       <c r="F5">
-        <v>0.80125996793817467</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+        <v>0.75062931986133785</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3291.4058438329862</v>
+        <v>1586.265755506038</v>
       </c>
       <c r="C6">
-        <v>203.90420383331545</v>
+        <v>316.59386294093133</v>
       </c>
       <c r="D6">
-        <v>200.93742684759431</v>
+        <v>299.17758909625786</v>
       </c>
       <c r="E6">
-        <v>29.981610447448098</v>
+        <v>25.339936746497376</v>
       </c>
       <c r="F6">
-        <v>0.7308472424080148</v>
-      </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
+        <v>0.73307436406368987</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>700.08890861459793</v>
+        <v>1427.9315626280095</v>
       </c>
       <c r="C7">
-        <v>260.50363872666151</v>
+        <v>182.27691176353696</v>
       </c>
       <c r="D7">
-        <v>159.13244547605649</v>
+        <v>309.01209466362548</v>
       </c>
       <c r="E7">
-        <v>21.471631467245636</v>
+        <v>38.408279724889667</v>
       </c>
       <c r="F7">
-        <v>0.73948219746198574</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
+        <v>0.67638968561799651</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1323.002416509358</v>
+        <v>1607.0850723645597</v>
       </c>
       <c r="C8">
-        <v>265.74777804915601</v>
+        <v>469.11380701858508</v>
       </c>
       <c r="D8">
-        <v>278.81993695844272</v>
+        <v>257.26634518543131</v>
       </c>
       <c r="E8">
-        <v>26.328284771888875</v>
+        <v>22.836473266377507</v>
       </c>
       <c r="F8">
-        <v>0.78692394589120906</v>
-      </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
+        <v>0.74110396471582696</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>5398.5952843189025</v>
+        <v>1016.0850193150385</v>
       </c>
       <c r="C9">
-        <v>143.08102578979185</v>
+        <v>597.75970461889665</v>
       </c>
       <c r="D9">
-        <v>257.45560691180901</v>
+        <v>321.92143326601422</v>
       </c>
       <c r="E9">
-        <v>28.850616618088992</v>
+        <v>24.597625046621566</v>
       </c>
       <c r="F9">
-        <v>0.80548443462759112</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
+        <v>0.80566507213112892</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>5480.0202189836009</v>
+        <v>803.9044086157628</v>
       </c>
       <c r="C10">
-        <v>651.04680205930629</v>
+        <v>183.13305392079258</v>
       </c>
       <c r="D10">
-        <v>301.14405364802047</v>
+        <v>235.05877114235346</v>
       </c>
       <c r="E10">
-        <v>23.239912428472213</v>
+        <v>34.996210824343436</v>
       </c>
       <c r="F10">
-        <v>0.82922058320070213</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
+        <v>0.74483897672326815</v>
+      </c>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1070.6126491482855</v>
+        <v>4544.3502977197568</v>
       </c>
       <c r="C11">
-        <v>172.44462683572397</v>
+        <v>134.98730414784328</v>
       </c>
       <c r="D11">
-        <v>190.24221909502398</v>
+        <v>235.50308096347112</v>
       </c>
       <c r="E11">
-        <v>37.904523562884144</v>
+        <v>36.98598846397546</v>
       </c>
       <c r="F11">
-        <v>0.65604679837832458</v>
-      </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
-      <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
+        <v>0.70881481192294182</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>1567.4072303121779</v>
+        <v>2148.5676445281911</v>
       </c>
       <c r="C12">
-        <v>241.67046531508313</v>
+        <v>261.45235357486433</v>
       </c>
       <c r="D12">
-        <v>337.3358178012133</v>
+        <v>273.31176914196158</v>
       </c>
       <c r="E12">
-        <v>23.966261931510935</v>
+        <v>29.282732792226795</v>
       </c>
       <c r="F12">
-        <v>0.68588583991886709</v>
-      </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
-      <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
+        <v>0.79763950567486819</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>2473.8786597755561</v>
+        <v>869.11390662411668</v>
       </c>
       <c r="C13">
-        <v>204.98338152100933</v>
+        <v>191.8646169726257</v>
       </c>
       <c r="D13">
-        <v>174.04595410640732</v>
+        <v>171.44093284295218</v>
       </c>
       <c r="E13">
-        <v>22.916900663124707</v>
+        <v>38.660637461690747</v>
       </c>
       <c r="F13">
-        <v>0.72129343355699682</v>
-      </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
-      <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
+        <v>0.77116223851088017</v>
+      </c>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>4933.1725743853603</v>
+        <v>2566.1869615825585</v>
       </c>
       <c r="C14">
-        <v>296.05187876438993</v>
+        <v>173.30637615947421</v>
       </c>
       <c r="D14">
-        <v>295.40236446207399</v>
+        <v>202.30296937560789</v>
       </c>
       <c r="E14">
-        <v>31.165307737448483</v>
+        <v>27.283278423061283</v>
       </c>
       <c r="F14">
-        <v>0.66783625110677336</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
-      <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
+        <v>0.77125802638963792</v>
+      </c>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>3791.2134980130254</v>
+        <v>3372.5878596785892</v>
       </c>
       <c r="C15">
-        <v>385.1654726155848</v>
+        <v>586.05334784517277</v>
       </c>
       <c r="D15">
-        <v>199.52031653584518</v>
+        <v>298.28630355201005</v>
       </c>
       <c r="E15">
-        <v>38.340135411326685</v>
+        <v>38.606197623736762</v>
       </c>
       <c r="F15">
-        <v>0.69185801145268422</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
+        <v>0.80163961854094479</v>
+      </c>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>2488.8028353943519</v>
+        <v>3245.1181674466648</v>
       </c>
       <c r="C16">
-        <v>325.04677113087155</v>
+        <v>152.01135139626564</v>
       </c>
       <c r="D16">
-        <v>274.15578297944711</v>
+        <v>236.63931585521385</v>
       </c>
       <c r="E16">
-        <v>39.50814782582605</v>
+        <v>23.816543202555252</v>
       </c>
       <c r="F16">
-        <v>0.81575667348539105</v>
-      </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
-      <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
+        <v>0.67892646100276455</v>
+      </c>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>3129.2907797441972</v>
+        <v>3130.8576137612904</v>
       </c>
       <c r="C17">
-        <v>424.44305697941962</v>
+        <v>267.29377908998339</v>
       </c>
       <c r="D17">
-        <v>253.41405113585009</v>
+        <v>163.68646858017703</v>
       </c>
       <c r="E17">
-        <v>38.329915907360586</v>
+        <v>23.759801068578334</v>
       </c>
       <c r="F17">
-        <v>0.73755669460277173</v>
-      </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
-      <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
+        <v>0.7947233740045937</v>
+      </c>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>4075.2833670031109</v>
+        <v>5453.9067716198824</v>
       </c>
       <c r="C18">
-        <v>396.10155397571481</v>
+        <v>265.7151011060817</v>
       </c>
       <c r="D18">
-        <v>208.35178943982257</v>
+        <v>269.97398576850128</v>
       </c>
       <c r="E18">
-        <v>36.835607322465449</v>
+        <v>36.087129719962007</v>
       </c>
       <c r="F18">
-        <v>0.746972916364672</v>
-      </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
+        <v>0.77909594725692388</v>
+      </c>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19">
-        <v>2455.1219692158365</v>
+        <v>5238.4822068353396</v>
       </c>
       <c r="C19">
-        <v>778.89620567670181</v>
+        <v>177.56892463493227</v>
       </c>
       <c r="D19">
-        <v>333.41742699230917</v>
+        <v>282.93038477272995</v>
       </c>
       <c r="E19">
-        <v>38.949619037929132</v>
+        <v>22.516096176388977</v>
       </c>
       <c r="F19">
-        <v>0.79804173390180921</v>
-      </c>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
+        <v>0.78738302683527461</v>
+      </c>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>664.02667935990155</v>
+        <v>3620.7391527509726</v>
       </c>
       <c r="C20">
-        <v>539.5368908169221</v>
+        <v>501.54273030448053</v>
       </c>
       <c r="D20">
-        <v>283.49775528403109</v>
+        <v>276.82882904334241</v>
       </c>
       <c r="E20">
-        <v>20.384885983378442</v>
+        <v>36.320800474486632</v>
       </c>
       <c r="F20">
-        <v>0.74907284133355234</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+        <v>0.78856875718677921</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>3208.6767938310345</v>
+        <v>2123.526235169993</v>
       </c>
       <c r="C21">
-        <v>217.97595828358675</v>
+        <v>269.50055472074854</v>
       </c>
       <c r="D21">
-        <v>189.44132888027761</v>
+        <v>303.89815693097523</v>
       </c>
       <c r="E21">
-        <v>24.801328841557574</v>
+        <v>21.737747267842032</v>
       </c>
       <c r="F21">
-        <v>0.69825853862338572</v>
-      </c>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+        <v>0.7885708613470459</v>
+      </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1180,6 +1198,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>